<commit_message>
completed several things! yay!!
</commit_message>
<xml_diff>
--- a/deliverables-checklist.xlsx
+++ b/deliverables-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\UIUC\Fall 2019\IS590 Open Data Mashups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC954D0-9FE7-4E8E-B923-72039B1732A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE4CEED-BAD6-4B12-9D13-75445F8ACFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA5DA797-928C-4257-AB81-5FADF6247F41}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>Shows which files contain all the checklist elements</t>
   </si>
   <si>
-    <t>TBD, will write when everything is organized and settled</t>
-  </si>
-  <si>
     <t>CSV file containing final data; produced with Jupyter Notebook</t>
   </si>
   <si>
@@ -108,42 +105,24 @@
     <t>For each dataset, the records that I'll use to form the final dataset are clean and ready for extraction. Each dataset also has its own versioning folder with different versions at fairly consistent stages.</t>
   </si>
   <si>
-    <t>At whatever stage of completion they were at when I completed the assignment; now that I'm done working with the datsets I can finish this</t>
-  </si>
-  <si>
     <t>in "data-documentation-files", .md files</t>
   </si>
   <si>
     <t>Commented and documented code for all data gathering you did using code.  Any hand created files should have detailed descriptions of their creation.</t>
   </si>
   <si>
-    <t>Need to add comments to code used for processing datasets; used code for ESTC, OTA, and gutenberg</t>
-  </si>
-  <si>
-    <t>Will add to dataset documentation files where relevant; put XPATH collection method notes here (definitely for open-syllabus, and some other dataset I think?)</t>
-  </si>
-  <si>
     <t>Jupyter Notebook</t>
   </si>
   <si>
     <t>A notebook with code to reproducibly create your final data file from your intermediate data files, with comments and narrative, suitable for a tutorial or demonstration.  I should be able to delete your final data fiile and recreate it based just off your intermediate data files and the code in this notebook.</t>
   </si>
   <si>
-    <t>Pretty much done - just have to add a couple lines to Jupyter Notebook to actually write out the csv file</t>
-  </si>
-  <si>
-    <t>Pretty sure this is done; idk if I'm confident with the dataframe results but it feels too late to redo my datasets for reprocessing - talk to Elizabeth? If Elizabeth says it's fine, need to add markdown cells ("describe you selection process and explain your thought process") and add a couple lines of code to write out the csv and we're done</t>
-  </si>
-  <si>
     <t>Github Repo</t>
   </si>
   <si>
     <t>contains everything above.  If you have data that’s too big to be stored in github, you’ll need to have it hosted in a box folder or something.</t>
   </si>
   <si>
-    <t>Chugging along; will also include link to Box folder with versioning and thousands of RDF files</t>
-  </si>
-  <si>
     <t>either submit an updated resume with this element highlighted or submit the text extract as a PDF</t>
   </si>
   <si>
@@ -178,6 +157,27 @@
   </si>
   <si>
     <t>lol fuck this</t>
+  </si>
+  <si>
+    <t>Used code for ESTC and gutenberg and added comments</t>
+  </si>
+  <si>
+    <t>added to "cleaning assessment" sections of individual dataset documentation files</t>
+  </si>
+  <si>
+    <t>MANIFEST.md (still missing resume entry, summary slide, assessment report)</t>
+  </si>
+  <si>
+    <t>it exists! final_dataset.csv</t>
+  </si>
+  <si>
+    <t>emailed elizabeth - if she gives the green light, this is done</t>
+  </si>
+  <si>
+    <t>change/add file names; wait for elizabeth to answer versioning question</t>
+  </si>
+  <si>
+    <t>updating as I go</t>
   </si>
 </sst>
 </file>
@@ -598,14 +598,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5298880-3336-4B55-9D5E-98295F129064}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.08984375" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="37.1796875" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
@@ -636,10 +636,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -653,10 +653,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -670,10 +670,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -694,10 +694,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -711,13 +711,13 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,92 +731,92 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="62" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -830,10 +830,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -847,10 +847,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -864,16 +864,19 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E17">
+    <sortCondition descending="1" ref="E7:E17"/>
+  </sortState>
   <conditionalFormatting sqref="E3:E17">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
checked off EVEN MORE STUFF! NICE!!
</commit_message>
<xml_diff>
--- a/deliverables-checklist.xlsx
+++ b/deliverables-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\UIUC\Fall 2019\IS590 Open Data Mashups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE4CEED-BAD6-4B12-9D13-75445F8ACFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EDC9CB-F431-4542-AB93-7227EE90CBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA5DA797-928C-4257-AB81-5FADF6247F41}"/>
   </bookViews>
@@ -165,26 +165,26 @@
     <t>added to "cleaning assessment" sections of individual dataset documentation files</t>
   </si>
   <si>
-    <t>MANIFEST.md (still missing resume entry, summary slide, assessment report)</t>
-  </si>
-  <si>
     <t>it exists! final_dataset.csv</t>
   </si>
   <si>
-    <t>emailed elizabeth - if she gives the green light, this is done</t>
-  </si>
-  <si>
-    <t>change/add file names; wait for elizabeth to answer versioning question</t>
-  </si>
-  <si>
     <t>updating as I go</t>
+  </si>
+  <si>
+    <t>green light from elizabeth! it's done!</t>
+  </si>
+  <si>
+    <t>pretty sure this is done!</t>
+  </si>
+  <si>
+    <t>MANIFEST.md (still missing file name identifiers for resume entry, summary slide, assessment report)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +202,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -260,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -282,6 +288,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5298880-3336-4B55-9D5E-98295F129064}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +695,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -748,7 +757,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="7">
         <v>2</v>
@@ -765,7 +774,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -781,14 +790,14 @@
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="155" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -802,10 +811,10 @@
         <v>46</v>
       </c>
       <c r="E13" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -816,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
made progress on conference talk proposal!
</commit_message>
<xml_diff>
--- a/deliverables-checklist.xlsx
+++ b/deliverables-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\UIUC\Fall 2019\IS590 Open Data Mashups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EDC9CB-F431-4542-AB93-7227EE90CBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD061FF3-998B-45CF-A248-4590BDAC4229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA5DA797-928C-4257-AB81-5FADF6247F41}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Final dataset file</t>
   </si>
@@ -147,18 +147,12 @@
     <t>lol shit</t>
   </si>
   <si>
-    <t>lol help</t>
-  </si>
-  <si>
     <t>intro, research question, high level data source overview, how data sources were combined, problems overcome, prelim results and discussion of value</t>
   </si>
   <si>
     <t>7-15 slides</t>
   </si>
   <si>
-    <t>lol fuck this</t>
-  </si>
-  <si>
     <t>Used code for ESTC and gutenberg and added comments</t>
   </si>
   <si>
@@ -178,6 +172,9 @@
   </si>
   <si>
     <t>MANIFEST.md (still missing file name identifiers for resume entry, summary slide, assessment report)</t>
+  </si>
+  <si>
+    <t>mostly done! Just need to write talk description</t>
   </si>
 </sst>
 </file>
@@ -607,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5298880-3336-4B55-9D5E-98295F129064}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,7 +642,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>35</v>
@@ -662,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>37</v>
@@ -682,10 +679,10 @@
         <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.35">
@@ -723,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
@@ -740,7 +737,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
@@ -757,7 +754,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="7">
         <v>2</v>
@@ -774,7 +771,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -791,7 +788,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="7">
         <v>2</v>
@@ -808,7 +805,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -825,7 +822,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -842,7 +839,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -859,7 +856,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
just a lil progress is still progress!
</commit_message>
<xml_diff>
--- a/deliverables-checklist.xlsx
+++ b/deliverables-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\UIUC\Fall 2019\IS590 Open Data Mashups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD061FF3-998B-45CF-A248-4590BDAC4229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D459F4-2F89-40C5-B2C3-CA6E5678A6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA5DA797-928C-4257-AB81-5FADF6247F41}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Final dataset file</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>mostly done! Just need to write talk description</t>
+  </si>
+  <si>
+    <t>some slides are done</t>
   </si>
 </sst>
 </file>
@@ -604,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5298880-3336-4B55-9D5E-98295F129064}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,254 +637,254 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E7" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="7">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="1">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="8" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>45</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="155" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="155" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E17">
-    <sortCondition descending="1" ref="E7:E17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E17">
+    <sortCondition ref="E5:E17"/>
   </sortState>
   <conditionalFormatting sqref="E3:E17">
     <cfRule type="colorScale" priority="1">

</xml_diff>